<commit_message>
events:cutie mark & holiday
</commit_message>
<xml_diff>
--- a/data/age.xlsx
+++ b/data/age.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="9180" windowHeight="7545"/>
+    <workbookView windowWidth="20490" windowHeight="7725"/>
   </bookViews>
   <sheets>
     <sheet name="age" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="87">
   <si>
     <t>$age</t>
   </si>
@@ -163,13 +163,118 @@
     <t>10039*50</t>
   </si>
   <si>
+    <t>10040*50</t>
+  </si>
+  <si>
+    <t>10041*50</t>
+  </si>
+  <si>
+    <t>10042*50</t>
+  </si>
+  <si>
+    <t>10043*50</t>
+  </si>
+  <si>
+    <t>10044*50</t>
+  </si>
+  <si>
+    <t>10045*50</t>
+  </si>
+  <si>
+    <t>10046*50</t>
+  </si>
+  <si>
+    <t>10047*50</t>
+  </si>
+  <si>
+    <t>10048*50</t>
+  </si>
+  <si>
+    <t>10049*50</t>
+  </si>
+  <si>
+    <t>10050*50</t>
+  </si>
+  <si>
+    <t>10051*50</t>
+  </si>
+  <si>
+    <t>10052*50</t>
+  </si>
+  <si>
+    <t>10053*50</t>
+  </si>
+  <si>
+    <t>10056*60</t>
+  </si>
+  <si>
+    <t>10057*60</t>
+  </si>
+  <si>
+    <t>10058*60</t>
+  </si>
+  <si>
+    <t>10059*60</t>
+  </si>
+  <si>
+    <t>10060*60</t>
+  </si>
+  <si>
+    <t>10061*60</t>
+  </si>
+  <si>
+    <t>10062*60</t>
+  </si>
+  <si>
+    <t>10063*60</t>
+  </si>
+  <si>
+    <t>10064*60</t>
+  </si>
+  <si>
+    <t>10065*60</t>
+  </si>
+  <si>
+    <t>10066*60</t>
+  </si>
+  <si>
+    <t>10067*60</t>
+  </si>
+  <si>
+    <t>10068*60</t>
+  </si>
+  <si>
     <t>8</t>
   </si>
   <si>
+    <t>10028*10</t>
+  </si>
+  <si>
+    <t>10054*50</t>
+  </si>
+  <si>
     <t>9</t>
   </si>
   <si>
-    <t>40000</t>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
   </si>
 </sst>
 </file>
@@ -177,9 +282,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
@@ -204,6 +309,29 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
@@ -218,7 +346,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -232,33 +367,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -278,22 +391,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="等线"/>
@@ -309,8 +406,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F3F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -324,24 +422,31 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="等线"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -368,7 +473,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -380,31 +605,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -416,91 +629,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -518,37 +647,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -562,17 +667,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -580,8 +679,34 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -610,21 +735,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -640,182 +750,177 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1141,10 +1246,10 @@
   </sheetPr>
   <dimension ref="A1:KG504"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.2166666666667" defaultRowHeight="44.4" customHeight="1"/>
@@ -3047,7 +3152,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" ht="15" customHeight="1" spans="1:20">
+    <row r="10" ht="15" customHeight="1" spans="1:47">
       <c r="A10" s="3" t="s">
         <v>35</v>
       </c>
@@ -3108,16 +3213,97 @@
       <c r="T10" s="3" t="s">
         <v>48</v>
       </c>
+      <c r="U10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="V10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="W10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="X10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC10" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF10" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG10" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH10" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI10" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ10" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK10" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AL10" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM10" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN10" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO10" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AP10" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AQ10" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AR10" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AS10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AT10" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AU10" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
-    <row r="11" ht="15" customHeight="1" spans="1:14">
+    <row r="11" ht="15" customHeight="1" spans="1:42">
       <c r="A11" s="3" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>37</v>
+        <v>77</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>38</v>
@@ -3152,23 +3338,1123 @@
       <c r="N11" s="3" t="s">
         <v>48</v>
       </c>
+      <c r="O11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q11" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="R11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="U11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="V11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="W11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="X11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z11" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA11" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB11" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC11" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD11" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE11" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF11" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG11" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH11" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI11" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ11" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AK11" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL11" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM11" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN11" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AO11" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AP11" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
-    <row r="12" ht="15" customHeight="1" spans="1:2">
+    <row r="12" ht="15" customHeight="1" spans="1:42">
       <c r="A12" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P12" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="Q12" s="3" t="s">
         <v>51</v>
       </c>
+      <c r="R12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="U12" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="V12" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="W12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="X12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z12" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA12" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB12" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC12" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD12" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE12" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF12" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG12" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH12" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI12" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ12" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AK12" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL12" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM12" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN12" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AO12" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AP12" s="3" t="s">
+        <v>75</v>
+      </c>
     </row>
-    <row r="13" ht="15" customHeight="1"/>
-    <row r="14" ht="15" customHeight="1"/>
-    <row r="15" ht="15" customHeight="1"/>
-    <row r="16" ht="15" customHeight="1"/>
-    <row r="17" ht="15" customHeight="1"/>
-    <row r="18" ht="15" customHeight="1"/>
-    <row r="19" ht="15" customHeight="1"/>
-    <row r="20" ht="15" customHeight="1"/>
+    <row r="13" ht="15" customHeight="1" spans="1:42">
+      <c r="A13" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q13" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S13" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T13" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="U13" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="V13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="W13" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="X13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z13" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA13" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB13" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC13" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE13" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF13" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG13" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH13" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI13" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ13" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AK13" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL13" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM13" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN13" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AO13" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AP13" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" ht="15" customHeight="1" spans="1:42">
+      <c r="A14" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="R14" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T14" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="U14" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="V14" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="W14" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="X14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y14" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z14" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA14" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB14" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC14" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD14" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE14" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF14" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG14" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH14" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI14" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ14" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AK14" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL14" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM14" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN14" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AO14" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AP14" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" ht="15" customHeight="1" spans="1:42">
+      <c r="A15" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="R15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S15" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T15" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="U15" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="V15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="W15" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="X15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y15" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z15" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA15" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB15" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC15" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD15" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE15" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF15" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG15" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH15" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI15" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ15" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AK15" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL15" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM15" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN15" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AO15" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AP15" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" ht="15" customHeight="1" spans="1:42">
+      <c r="A16" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="R16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="U16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="V16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="W16" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="X16" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y16" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z16" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA16" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB16" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC16" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD16" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE16" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF16" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG16" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH16" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ16" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AK16" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL16" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM16" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN16" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AO16" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AP16" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" ht="15" customHeight="1" spans="1:42">
+      <c r="A17" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P17" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q17" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="R17" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S17" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T17" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="U17" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="V17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="W17" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="X17" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y17" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z17" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA17" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB17" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC17" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE17" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF17" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG17" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH17" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ17" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AK17" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL17" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM17" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN17" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AO17" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AP17" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" ht="15" customHeight="1" spans="1:42">
+      <c r="A18" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="N18" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="O18" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="R18" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S18" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T18" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="U18" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="V18" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="W18" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="X18" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y18" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z18" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA18" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB18" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC18" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD18" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE18" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF18" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG18" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH18" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ18" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AK18" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL18" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM18" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN18" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AO18" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AP18" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" ht="15" customHeight="1" spans="1:42">
+      <c r="A19" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="N19" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="O19" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P19" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q19" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="R19" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S19" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="T19" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="U19" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="V19" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="W19" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="X19" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y19" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z19" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA19" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB19" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC19" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD19" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE19" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF19" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG19" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH19" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ19" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AK19" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL19" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM19" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN19" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AO19" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AP19" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" ht="15" customHeight="1" spans="1:2">
+      <c r="A20" s="3">
+        <v>17</v>
+      </c>
+      <c r="B20" s="3">
+        <v>40000</v>
+      </c>
+    </row>
     <row r="21" ht="15" customHeight="1"/>
     <row r="22" ht="15" customHeight="1"/>
     <row r="23" ht="15" customHeight="1"/>

</xml_diff>